<commit_message>
renames folders, creation user historys, project organization
</commit_message>
<xml_diff>
--- a/documentacion/bitacora_iteraciones_template.xlsx
+++ b/documentacion/bitacora_iteraciones_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\bici-go-bd\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6ACEB36-95A5-428C-BD1C-5B0D9A1F767F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8596D4F6-54FA-4A13-9756-04A019FF4EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Iteración</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Rama (feature/*)</t>
   </si>
   <si>
-    <t>Alcance (conceptual/lógico/físico)</t>
-  </si>
-  <si>
     <t>Autor</t>
   </si>
   <si>
@@ -58,73 +55,43 @@
     <t>Estado (Planificado/En curso/Completado)</t>
   </si>
   <si>
-    <t>Evidencias (links)</t>
-  </si>
-  <si>
     <t>Archivos afectados (ruta)</t>
   </si>
   <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>1.1</t>
-  </si>
-  <si>
     <t>H1 – Bicicletas</t>
   </si>
   <si>
-    <t>feature/h1-bicicletas-conceptual</t>
-  </si>
-  <si>
-    <t>feature/h1-ajuste-kilometraje</t>
-  </si>
-  <si>
-    <t>conceptual</t>
-  </si>
-  <si>
-    <t>lógico</t>
-  </si>
-  <si>
     <t>andr4f</t>
   </si>
   <si>
-    <t>nombre_revisor</t>
-  </si>
-  <si>
-    <t>https://github.com/andr4f/bici-go-bd/pull/12</t>
-  </si>
-  <si>
-    <t>https://github.com/andr4f/bici-go-bd/pull/15</t>
-  </si>
-  <si>
-    <t>v0.1-iter1</t>
-  </si>
-  <si>
-    <t>v0.1.1-h1-ajuste</t>
-  </si>
-  <si>
-    <t>E-R inicial; entidades Bicicleta/TipoUso/TipoAsistencia</t>
-  </si>
-  <si>
-    <t>Agregar atributo kilometraje + CHECK</t>
-  </si>
-  <si>
-    <t>2025-09-27</t>
-  </si>
-  <si>
-    <t>2025-09-28</t>
-  </si>
-  <si>
     <t>Completado</t>
   </si>
   <si>
-    <t>modelos/conceptual/er_bicicletas.drawio</t>
-  </si>
-  <si>
-    <t>modelos/logico/der_relacional.pdf</t>
-  </si>
-  <si>
-    <t>sql/iteracion_02/01_alter_add_kilometraje.sql</t>
+    <t>feature/creacion_historias_usuario</t>
+  </si>
+  <si>
+    <t>creacion_de_historias</t>
+  </si>
+  <si>
+    <t>Alcance (conceptual/lógico/físico/creacion_de_historias)</t>
+  </si>
+  <si>
+    <t>Yineth Avila, Angel Trillo, Andres Penagos</t>
+  </si>
+  <si>
+    <t>v0.1-iter1-creacion</t>
+  </si>
+  <si>
+    <t>documentacion/back_logs_historias_usuario/sub_historias_h1/primeras_tres_sub_historias.pdf</t>
+  </si>
+  <si>
+    <t>Creacion primeras 3 historias de usuario a partir de H1 principal</t>
+  </si>
+  <si>
+    <t>https://github.com/andr4f/bici-go-bd/pull/3</t>
   </si>
 </sst>
 </file>
@@ -194,12 +161,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -541,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,7 +518,7 @@
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.77734375" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
     <col min="7" max="7" width="46.6640625" customWidth="1"/>
@@ -558,8 +526,8 @@
     <col min="9" max="9" width="57.6640625" customWidth="1"/>
     <col min="10" max="11" width="14.6640625" customWidth="1"/>
     <col min="12" max="12" width="42.6640625" customWidth="1"/>
-    <col min="13" max="13" width="41.6640625" customWidth="1"/>
-    <col min="14" max="14" width="47.6640625" customWidth="1"/>
+    <col min="13" max="13" width="81" customWidth="1"/>
+    <col min="14" max="14" width="78.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -573,131 +541,84 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="J2" s="3">
+        <v>45933</v>
+      </c>
+      <c r="K2" s="3">
+        <v>45933</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
+      <c r="G3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{29AA7A1E-9A5B-411F-9740-018B94C7EA1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
creacion modelo conceptual iteracion 2
</commit_message>
<xml_diff>
--- a/documentacion/bitacora_iteraciones_template.xlsx
+++ b/documentacion/bitacora_iteraciones_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\bici_go_bd\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA985B5E-D943-4949-A1B7-8909F51CF826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8695553-8379-44D1-A5A8-346F620ADB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>Iteración</t>
   </si>
@@ -194,6 +194,21 @@
   </si>
   <si>
     <t>documentacion/backlog_historias_usuario/sub_historias_h1</t>
+  </si>
+  <si>
+    <t>feature/modelo_conceptual_iter_2</t>
+  </si>
+  <si>
+    <t>https://github.com/andr4f/bici-go-bd/pull/13</t>
+  </si>
+  <si>
+    <t>v0.2-iter2-conceptual</t>
+  </si>
+  <si>
+    <t>Creacion modelo conceptual iteracion 2</t>
+  </si>
+  <si>
+    <t>bici_go_bd/modelos/conceptual/iteracion_2</t>
   </si>
 </sst>
 </file>
@@ -610,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,12 +936,54 @@
         <v>57</v>
       </c>
     </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="4">
+        <v>45942</v>
+      </c>
+      <c r="K8" s="4">
+        <v>45942</v>
+      </c>
+      <c r="L8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{3B7A025C-D54F-423D-8940-9A69AB9B1AA0}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{02D14F77-4C92-4034-BDA2-19B8ACA38146}"/>
     <hyperlink ref="G6" r:id="rId3" xr:uid="{B4CEFF8D-DDDE-4135-86C8-D93E07F2D697}"/>
     <hyperlink ref="G7" r:id="rId4" xr:uid="{7B166655-AC2F-4E1E-9B2E-B2C09BE9DBB0}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{2FC91176-81F3-44DC-BD63-6B5F1C8E12C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizacion de glosario y alcance
</commit_message>
<xml_diff>
--- a/documentacion/bitacora_iteraciones_template.xlsx
+++ b/documentacion/bitacora_iteraciones_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USAURIO\bici-go-bd\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\bici-go-bd\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BAFF98-5316-45BD-8D97-53DF9DD58263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC37E624-992E-43AB-9A65-D43ABB0D7B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitacora" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Iteración</t>
   </si>
@@ -248,6 +248,24 @@
   </si>
   <si>
     <t>bici_go_bd/modelos/fisico/iteracion_2</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>feature/creacion_historias_usuario_iter_3</t>
+  </si>
+  <si>
+    <t>https://github.com/andr4f/bici-go-bd/pull/16</t>
+  </si>
+  <si>
+    <t>v0.1-iter3-creacion</t>
+  </si>
+  <si>
+    <t>Creacion de 4 historias mas para completar 10, creacion de glosario y alcance de datos</t>
+  </si>
+  <si>
+    <t>documentacion/backlog_historias_usuario/</t>
   </si>
 </sst>
 </file>
@@ -667,28 +685,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="57.7109375" customWidth="1"/>
-    <col min="10" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="73.109375" customWidth="1"/>
+    <col min="10" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="42.6640625" customWidth="1"/>
     <col min="13" max="13" width="81" customWidth="1"/>
-    <col min="14" max="14" width="78.5703125" customWidth="1"/>
+    <col min="14" max="14" width="78.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +748,7 @@
       </c>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -771,7 +789,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -812,7 +830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -853,7 +871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -894,7 +912,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -935,7 +953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -976,7 +994,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1017,7 +1035,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1058,7 +1076,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1099,7 +1117,48 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="4">
+        <v>45944</v>
+      </c>
+      <c r="K11" s="4">
+        <v>45945</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M12" s="5"/>
     </row>
   </sheetData>
@@ -1111,8 +1170,9 @@
     <hyperlink ref="G8" r:id="rId5" xr:uid="{2FC91176-81F3-44DC-BD63-6B5F1C8E12C4}"/>
     <hyperlink ref="G9" r:id="rId6" xr:uid="{098972D2-BD7A-4375-BA04-41D3B4AA47FD}"/>
     <hyperlink ref="G10" r:id="rId7" xr:uid="{9B0DD17D-E8B4-4021-8258-6728B626103E}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{6330800C-E47B-4EDC-86E4-1378D6CAC5C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correciones conceptual,  implementacion conceptual historias 7,8,9,10
</commit_message>
<xml_diff>
--- a/documentacion/bitacora_iteraciones_template.xlsx
+++ b/documentacion/bitacora_iteraciones_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilan\bici-go-bd\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEBC614-80FE-4821-A70F-4A15044CF077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B9C1D0-22C9-4241-8720-6A52659AE314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -666,7 +666,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1167,7 @@
         <v>45946</v>
       </c>
       <c r="K12" s="4">
-        <v>45948</v>
+        <v>45949</v>
       </c>
       <c r="L12" t="s">
         <v>15</v>

</xml_diff>